<commit_message>
[InvolvingFeatures] update experimental results for GPL
</commit_message>
<xml_diff>
--- a/experiment_results/INVOLVING_FEATURES/GPL/4wise/4wise-GPL-IF.xlsx
+++ b/experiment_results/INVOLVING_FEATURES/GPL/4wise/4wise-GPL-IF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuanngokien/Desktop/Software_Analysis/configurable_system/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tuanngokien/Desktop/Software_Analysis/configurable_system/InputPreparation/experiment_results/INVOLVING_FEATURES/GPL/4wise/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EB5AC59-E5B2-EA49-9C67-70BC33648AD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBC3DEC-7BD1-3B47-BF82-B1BD66042D53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="2860" windowWidth="27240" windowHeight="16440" xr2:uid="{B3559EE4-8399-C348-A2CB-8BF475FA5933}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{B3559EE4-8399-C348-A2CB-8BF475FA5933}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$91</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="232">
   <si>
     <t>MUTATED_PROJECT</t>
   </si>
@@ -501,241 +501,229 @@
     <t>NUM OF INVOLVING FEATURES</t>
   </si>
   <si>
-    <t>["Number", "DFS", "Weighted", "BFS", "TestProg", "MSTKruskal", "DirectedOnlyVertices", "UndirectedWithEdges"]</t>
-  </si>
-  <si>
-    <t>["Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Number", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WithNeighbors", "WeightedWithEdges", "Connected", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "BFS", "TestProg", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "Weighted", "UndirectedOnlyVertices", "Cycle", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Number", "UndirectedOnlyVertices", "Cycle", "MSTPrim", "UndirectedWithNeighbors", "BFS", "MSTKruskal", "DirectedWithEdges", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "DirectedOnlyVertices", "StronglyConnected"]</t>
-  </si>
-  <si>
     <t>["Cycle"]</t>
   </si>
   <si>
-    <t>["WeightedWithNeighbors", "Number", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "BFS", "MSTKruskal", "DirectedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "DirectedOnlyVertices", "StronglyConnected"]</t>
-  </si>
-  <si>
     <t>["Cycle", "Transpose"]</t>
   </si>
   <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["OnlyVertices", "Undirected", "Number", "Weighted", "Cycle", "BFS", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "WeightedOnlyVertices", "Connected", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Cycle", "MSTKruskal", "Unweighted", "WithNeighbors", "DirectedWithEdges", "DirectedOnlyVertices", "Transpose", "UndirectedWithEdges"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "Cycle", "BFS", "DirectedWithEdges", "Connected", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "Weighted", "Cycle", "BFS", "Unweighted", "WithNeighbors", "WithEdges", "Connected", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "BFS", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "Weighted", "Cycle", "TestProg", "BFS", "Unweighted", "DirectedWithEdges", "WeightedWithEdges", "Connected", "DirectedOnlyVertices", "StronglyConnected", "DirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["Number", "Weighted", "Cycle", "BFS", "TestProg", "WithEdges", "Connected", "Transpose"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "DirectedWithEdges", "WithNeighbors", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "WeightedOnlyVertices", "Connected", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "DirectedWithEdges", "Unweighted", "Connected", "Transpose", "UndirectedWithEdges", "StronglyConnected", "DirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "BFS", "Connected", "MSTKruskal", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "BFS", "TestProg", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "BFS", "TestProg", "WithNeighbors", "DirectedWithEdges", "Unweighted", "WithEdges", "DirectedOnlyVertices", "DFS", "OnlyVertices", "Weighted", "UndirectedOnlyVertices", "Cycle", "WeightedOnlyVertices", "Transpose", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["OnlyVertices", "Undirected", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "DirectedWithEdges", "Unweighted", "WeightedWithEdges", "WithEdges", "Connected", "UndirectedWithEdges", "DirectedOnlyVertices", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["UndirectedWithNeighbors", "BFS", "MSTKruskal", "DirectedWithEdges", "WithNeighbors", "Unweighted", "Connected", "UndirectedWithEdges", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
-    <t>["Number", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "BFS", "MSTKruskal", "DirectedWithEdges", "WithNeighbors", "Unweighted", "WeightedWithEdges", "Connected", "UndirectedWithEdges", "DirectedOnlyVertices", "StronglyConnected", "DirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "TestProg", "BFS", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "DirectedWithNeighbors", "OnlyVertices", "Weighted", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
     <t>["MSTKruskal"]</t>
   </si>
   <si>
-    <t>["Undirected", "Number", "MSTPrim", "TestProg", "BFS", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "Undirected", "MSTPrim", "BFS", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedWithNeighbors", "OnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "MSTPrim", "TestProg", "DirectedWithEdges", "Unweighted", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "BFS", "TestProg", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "WeightedOnlyVertices", "Connected", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "BFS", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "BFS", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "OnlyVertices", "Weighted", "UndirectedOnlyVertices", "UndirectedWithNeighbors", "WeightedOnlyVertices", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Unweighted", "Weighted", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "BFS", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "OnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "WeightedWithEdges", "WeightedOnlyVertices", "Connected", "UndirectedWithEdges", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "UndirectedWithNeighbors", "DirectedWithEdges", "Unweighted", "WeightedWithEdges", "WithEdges", "UndirectedWithEdges", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "TestProg", "BFS", "DirectedWithEdges", "WithNeighbors", "Unweighted", "WithEdges", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Number", "MSTPrim", "BFS", "WithNeighbors", "DirectedWithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "Weighted", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "BFS", "MSTKruskal", "DirectedWithEdges", "WithNeighbors", "WeightedWithEdges", "Connected", "Transpose", "UndirectedWithEdges"]</t>
-  </si>
-  <si>
-    <t>["Transpose", "DirectedWithEdges", "Unweighted", "DirectedOnlyVertices", "UndirectedWithNeighbors", "UndirectedWithEdges"]</t>
-  </si>
-  <si>
-    <t>["OnlyVertices", "Undirected", "Number", "Weighted", "MSTPrim", "Cycle", "UndirectedWithNeighbors", "Directed", "TestProg", "DirectedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
-    <t>["Transpose", "WeightedOnlyVertices", "DirectedOnlyVertices", "UndirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["Number", "UndirectedOnlyVertices", "Cycle", "MSTPrim", "UndirectedWithNeighbors", "UndirectedWithEdges", "DirectedWithEdges", "WeightedOnlyVertices", "Connected", "Transpose", "DFS", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
-    <t>["Transpose", "Undirected", "WeightedOnlyVertices", "DirectedOnlyVertices", "UndirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithEdges", "DirectedOnlyVertices", "UndirectedWithNeighbors", "BFS"]</t>
-  </si>
-  <si>
-    <t>["BFS", "WeightedWithEdges", "Connected", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "MSTPrim", "TestProg", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DFS", "OnlyVertices", "Weighted", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "MSTKruskal", "WeightedWithEdges", "Connected", "Transpose", "Directed"]</t>
-  </si>
-  <si>
-    <t>["UndirectedOnlyVertices", "WeightedWithEdges", "DirectedOnlyVertices", "Connected", "UndirectedWithNeighbors", "BFS"]</t>
-  </si>
-  <si>
-    <t>["Number", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "BFS", "MSTKruskal", "WeightedWithEdges", "Connected", "DirectedOnlyVertices", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["Undirected", "Number", "BFS", "TestProg", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "MSTKruskal", "WeightedWithEdges", "Connected", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
     <t>["DirectedOnlyVertices", "BFS", "WeightedWithEdges"]</t>
   </si>
   <si>
-    <t>["WeightedWithNeighbors", "Number", "UndirectedOnlyVertices", "Cycle", "MSTPrim", "BFS", "DirectedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "Undirected", "MSTPrim", "BFS", "DirectedWithEdges", "Unweighted", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "Connected", "Transpose", "UndirectedWithEdges", "Directed"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "UndirectedOnlyVertices", "DirectedOnlyVertices", "UndirectedWithNeighbors", "UndirectedWithEdges"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Unweighted", "WithEdges", "DirectedOnlyVertices", "Transpose"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Undirected", "Number", "MSTPrim", "BFS", "TestProg", "Unweighted", "DirectedWithEdges", "WithNeighbors", "WithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "UndirectedOnlyVertices", "MSTPrim", "Cycle", "BFS", "WithEdges", "DirectedOnlyVertices", "UndirectedWithEdges", "StronglyConnected", "DirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "UndirectedOnlyVertices", "UndirectedWithNeighbors", "BFS"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "UndirectedOnlyVertices", "Cycle", "DirectedWithEdges", "Connected", "Transpose", "UndirectedWithEdges", "DirectedOnlyVertices", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Transpose", "DirectedOnlyVertices"]</t>
-  </si>
-  <si>
     <t>["WeightedWithNeighbors", "DirectedOnlyVertices"]</t>
   </si>
   <si>
-    <t>["WeightedWithNeighbors", "Number", "Undirected", "MSTPrim", "TestProg", "Unweighted", "WithNeighbors", "DirectedWithEdges", "WithEdges", "DirectedOnlyVertices", "DirectedWithNeighbors", "UndirectedOnlyVertices", "Weighted", "Cycle", "UndirectedWithNeighbors", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "UndirectedOnlyVertices", "Weighted", "DirectedWithEdges", "WithEdges", "Transpose", "UndirectedWithEdges", "DirectedWithNeighbors"]</t>
-  </si>
-  <si>
-    <t>["WeightedWithNeighbors", "Number", "MSTPrim", "BFS", "DirectedWithEdges", "DirectedOnlyVertices", "DFS", "DirectedWithNeighbors", "OnlyVertices", "UndirectedOnlyVertices", "Cycle", "UndirectedWithNeighbors", "Connected", "Transpose", "UndirectedWithEdges", "Directed", "StronglyConnected"]</t>
-  </si>
-  <si>
     <t>BUGGY STATEMENTS</t>
+  </si>
+  <si>
+    <t>["BFS", "Weighted", "TestProg", "UndirectedWithEdges", "Number", "MSTKruskal", "DFS", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Connected", "Number", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "WithNeighbors", "UndirectedWithNeighbors", "Connected", "Number", "MSTKruskal", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "Directed", "MSTPrim", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DFS", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "WeightedWithEdges", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "Transpose", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "StronglyConnected", "DirectedWithEdges", "MSTKruskal", "DirectedOnlyVertices", "MSTPrim", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "Transpose", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "StronglyConnected", "DirectedWithEdges", "MSTKruskal", "WeightedWithNeighbors", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "WeightedWithEdges", "Cycle", "WeightedOnlyVertices", "UndirectedOnlyVertices", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithNeighbors", "WithEdges", "Unweighted", "Undirected", "Connected", "Weighted", "Number", "StronglyConnected", "DirectedWithEdges", "Directed", "OnlyVertices", "WeightedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "WithNeighbors", "Transpose", "Unweighted", "Undirected", "UndirectedWithEdges", "DirectedWithEdges", "MSTKruskal", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "Connected", "Number", "DirectedWithEdges", "WeightedWithNeighbors", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithNeighbors", "WithEdges", "Unweighted", "Undirected", "Connected", "Weighted", "Number", "Directed"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "Unweighted", "Connected", "Weighted", "TestProg", "Number", "StronglyConnected", "DirectedWithNeighbors", "DirectedWithEdges", "WeightedWithNeighbors", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithEdges", "Transpose", "Connected", "Weighted", "TestProg", "Number"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Weighted", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WithNeighbors", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "Transpose", "UndirectedWithNeighbors", "Unweighted", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "StronglyConnected", "DirectedWithNeighbors", "DirectedWithEdges", "MSTKruskal", "WeightedWithNeighbors"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithEdges", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Connected", "DirectedWithEdges", "MSTKruskal", "DirectedOnlyVertices", "Directed"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "Directed", "MSTPrim", "WeightedOnlyVertices", "Cycle", "WithNeighbors", "WithEdges", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Weighted", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedWithEdges", "Cycle", "WithEdges", "UndirectedOnlyVertices", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "Unweighted", "UndirectedOnlyVertices", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "UndirectedWithNeighbors", "Unweighted", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "StronglyConnected", "DirectedWithEdges", "MSTKruskal", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["BFS", "WithNeighbors", "UndirectedWithNeighbors", "Unweighted", "Connected", "UndirectedWithEdges", "DirectedWithEdges", "MSTKruskal", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithNeighbors", "UndirectedWithNeighbors", "Unweighted", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "StronglyConnected", "DirectedWithNeighbors", "DirectedWithEdges", "MSTKruskal", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["DirectedWithNeighbors", "WithEdges", "UndirectedWithNeighbors", "Transpose", "DirectedWithEdges", "UndirectedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "Directed", "MSTPrim", "WeightedWithEdges", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "Connected", "TestProg", "UndirectedWithEdges", "Number", "DirectedWithNeighbors", "DirectedWithEdges", "MSTKruskal", "MSTPrim", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "Unweighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "WeightedWithNeighbors", "Directed", "MSTPrim", "WeightedWithEdges", "Cycle", "WeightedOnlyVertices", "UndirectedOnlyVertices", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "Unweighted", "Weighted", "UndirectedWithEdges", "WeightedWithNeighbors", "Directed", "WeightedOnlyVertices", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "WeightedWithNeighbors", "WeightedOnlyVertices", "Cycle", "WeightedWithEdges", "WithNeighbors", "WithEdges", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["StronglyConnected", "UndirectedWithNeighbors", "Unweighted", "DirectedWithEdges", "DirectedOnlyVertices", "Weighted"]</t>
+  </si>
+  <si>
+    <t>["StronglyConnected", "Weighted", "Unweighted"]</t>
+  </si>
+  <si>
+    <t>["WithEdges", "UndirectedWithNeighbors", "Unweighted", "Undirected", "UndirectedWithEdges", "StronglyConnected", "DirectedWithEdges", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "TestProg", "Weighted", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "MSTPrim", "WeightedWithEdges", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "Directed", "MSTPrim", "WeightedWithEdges", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "UndirectedWithEdges", "DirectedWithNeighbors", "MSTKruskal", "Directed", "MSTPrim", "WeightedWithEdges", "Cycle", "WithNeighbors", "UndirectedOnlyVertices", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithNeighbors", "Transpose", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Undirected", "Connected", "Weighted", "UndirectedWithEdges", "Number", "DirectedWithEdges", "MSTKruskal", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "Unweighted", "DirectedWithEdges", "DirectedOnlyVertices", "UndirectedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "MSTPrim", "Transpose", "UndirectedWithNeighbors", "Undirected", "Connected", "Weighted", "TestProg", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "Directed", "OnlyVertices", "WeightedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "DirectedOnlyVertices", "WeightedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "Transpose", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "MSTPrim", "WeightedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "Undirected", "DirectedOnlyVertices", "WeightedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Connected", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "MSTKruskal", "Directed", "MSTPrim", "WeightedWithEdges", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Connected", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "Connected", "Number", "StronglyConnected", "MSTKruskal", "DirectedOnlyVertices", "WeightedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["BFS", "TestProg", "UndirectedWithEdges", "MSTKruskal", "Directed", "WeightedWithEdges", "Cycle", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "Transpose", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "DirectedWithNeighbors", "DirectedWithEdges", "WeightedWithNeighbors", "DirectedOnlyVertices", "MSTPrim"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "Unweighted", "Weighted", "UndirectedWithEdges", "DirectedWithNeighbors", "WeightedWithNeighbors", "Directed", "MSTPrim", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "DirectedWithEdges", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["UndirectedWithNeighbors", "UndirectedOnlyVertices", "WeightedWithNeighbors", "DirectedOnlyVertices", "UndirectedWithEdges"]</t>
+  </si>
+  <si>
+    <t>["WithEdges", "Transpose", "Unweighted", "WeightedWithNeighbors", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "Unweighted", "Weighted", "TestProg", "UndirectedWithEdges", "DirectedWithNeighbors", "WeightedWithNeighbors", "Directed", "MSTPrim", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "BFS", "WithEdges", "UndirectedOnlyVertices", "UndirectedWithEdges", "StronglyConnected", "DirectedWithNeighbors", "WeightedWithNeighbors", "DirectedOnlyVertices", "MSTPrim"]</t>
+  </si>
+  <si>
+    <t>["BFS", "UndirectedWithNeighbors", "UndirectedOnlyVertices", "WeightedWithNeighbors"]</t>
+  </si>
+  <si>
+    <t>["Cycle", "Transpose", "UndirectedOnlyVertices", "Connected", "UndirectedWithEdges", "Number", "StronglyConnected", "DirectedWithEdges", "WeightedWithNeighbors", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["WeightedWithNeighbors", "DirectedOnlyVertices", "Transpose"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "UndirectedWithNeighbors", "Unweighted", "TestProg", "Weighted", "UndirectedWithEdges", "DirectedWithNeighbors", "WeightedWithNeighbors", "Directed", "MSTPrim", "Cycle", "WithNeighbors", "WithEdges", "UndirectedOnlyVertices", "Undirected", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DirectedOnlyVertices"]</t>
+  </si>
+  <si>
+    <t>["Transpose", "WithEdges", "UndirectedOnlyVertices", "Weighted", "UndirectedWithEdges", "Number", "DirectedWithNeighbors", "DirectedWithEdges", "WeightedWithNeighbors"]</t>
+  </si>
+  <si>
+    <t>["BFS", "Transpose", "UndirectedWithNeighbors", "UndirectedWithEdges", "DirectedWithNeighbors", "WeightedWithNeighbors", "Directed", "MSTPrim", "Cycle", "UndirectedOnlyVertices", "Connected", "Number", "StronglyConnected", "DirectedWithEdges", "DFS", "DirectedOnlyVertices", "OnlyVertices"]</t>
   </si>
 </sst>
 </file>
@@ -1097,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E395AF-825B-D247-8D52-E7FE437DAB63}">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1119,7 +1107,7 @@
         <v>156</v>
       </c>
       <c r="D1" t="s">
-        <v>235</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1160,7 +1148,7 @@
         <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="C2">
         <f>LEN(B2)-LEN(SUBSTITUTE(B2,",","")) + 1</f>
@@ -1208,7 +1196,7 @@
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C66" si="0">LEN(B3)-LEN(SUBSTITUTE(B3,",","")) + 1</f>
@@ -1256,7 +1244,7 @@
         <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -1304,7 +1292,7 @@
         <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -1352,7 +1340,7 @@
         <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -1400,7 +1388,7 @@
         <v>124</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -1448,7 +1436,7 @@
         <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -1496,7 +1484,7 @@
         <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -1544,7 +1532,7 @@
         <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -1592,7 +1580,7 @@
         <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -1640,7 +1628,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -1688,7 +1676,7 @@
         <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -1736,7 +1724,7 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -1784,7 +1772,7 @@
         <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -1832,7 +1820,7 @@
         <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -1880,7 +1868,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -1928,7 +1916,7 @@
         <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -1976,7 +1964,7 @@
         <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
@@ -2024,7 +2012,7 @@
         <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
@@ -2072,7 +2060,7 @@
         <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -2120,7 +2108,7 @@
         <v>141</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
@@ -2168,7 +2156,7 @@
         <v>65</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
@@ -2216,7 +2204,7 @@
         <v>116</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
@@ -2264,7 +2252,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
@@ -2312,7 +2300,7 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
@@ -2360,7 +2348,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
@@ -2408,7 +2396,7 @@
         <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
@@ -2456,7 +2444,7 @@
         <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
@@ -2504,7 +2492,7 @@
         <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
@@ -2552,7 +2540,7 @@
         <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
@@ -2600,7 +2588,7 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
@@ -2648,7 +2636,7 @@
         <v>146</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
@@ -2696,7 +2684,7 @@
         <v>117</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
@@ -2744,7 +2732,7 @@
         <v>152</v>
       </c>
       <c r="B35" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
@@ -2792,7 +2780,7 @@
         <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
@@ -2840,7 +2828,7 @@
         <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
@@ -2888,7 +2876,7 @@
         <v>108</v>
       </c>
       <c r="B38" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
@@ -2936,7 +2924,7 @@
         <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
@@ -2984,7 +2972,7 @@
         <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
@@ -3032,7 +3020,7 @@
         <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
@@ -3080,11 +3068,11 @@
         <v>148</v>
       </c>
       <c r="B42" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
         <v>149</v>
@@ -3128,11 +3116,11 @@
         <v>134</v>
       </c>
       <c r="B43" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D43" t="s">
         <v>135</v>
@@ -3176,11 +3164,11 @@
         <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D44" t="s">
         <v>101</v>
@@ -3224,7 +3212,7 @@
         <v>122</v>
       </c>
       <c r="B45" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
@@ -3272,7 +3260,7 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
@@ -3320,11 +3308,11 @@
         <v>142</v>
       </c>
       <c r="B47" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="D47" t="s">
         <v>143</v>
@@ -3368,7 +3356,7 @@
         <v>61</v>
       </c>
       <c r="B48" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
@@ -3416,7 +3404,7 @@
         <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
@@ -3464,11 +3452,11 @@
         <v>126</v>
       </c>
       <c r="B50" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D50" t="s">
         <v>47</v>
@@ -3512,7 +3500,7 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
@@ -3564,7 +3552,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
         <v>47</v>
@@ -3660,7 +3648,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D54" t="s">
         <v>55</v>
@@ -3708,7 +3696,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
         <v>154</v>
@@ -3756,7 +3744,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D56" t="s">
         <v>55</v>
@@ -3848,7 +3836,7 @@
         <v>87</v>
       </c>
       <c r="B58" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
@@ -3896,7 +3884,7 @@
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
@@ -3944,7 +3932,7 @@
         <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
@@ -3992,7 +3980,7 @@
         <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
@@ -4040,7 +4028,7 @@
         <v>132</v>
       </c>
       <c r="B62" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
@@ -4088,7 +4076,7 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
@@ -4136,7 +4124,7 @@
         <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
@@ -4184,7 +4172,7 @@
         <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
@@ -4232,7 +4220,7 @@
         <v>114</v>
       </c>
       <c r="B66" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
@@ -4280,7 +4268,7 @@
         <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C67">
         <f t="shared" ref="C67:C91" si="1">LEN(B67)-LEN(SUBSTITUTE(B67,",","")) + 1</f>
@@ -4328,7 +4316,7 @@
         <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -4376,7 +4364,7 @@
         <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -4424,7 +4412,7 @@
         <v>150</v>
       </c>
       <c r="B70" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -4472,7 +4460,7 @@
         <v>92</v>
       </c>
       <c r="B71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -4520,7 +4508,7 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -4568,7 +4556,7 @@
         <v>109</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -4616,7 +4604,7 @@
         <v>129</v>
       </c>
       <c r="B74" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -4664,7 +4652,7 @@
         <v>31</v>
       </c>
       <c r="B75" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -4712,7 +4700,7 @@
         <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -4760,7 +4748,7 @@
         <v>130</v>
       </c>
       <c r="B77" t="s">
-        <v>221</v>
+        <v>160</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -4808,7 +4796,7 @@
         <v>59</v>
       </c>
       <c r="B78" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -4856,7 +4844,7 @@
         <v>133</v>
       </c>
       <c r="B79" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -4904,7 +4892,7 @@
         <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -4952,7 +4940,7 @@
         <v>147</v>
       </c>
       <c r="B81" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -5000,7 +4988,7 @@
         <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -5048,7 +5036,7 @@
         <v>20</v>
       </c>
       <c r="B83" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -5096,7 +5084,7 @@
         <v>145</v>
       </c>
       <c r="B84" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -5144,7 +5132,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
@@ -5192,7 +5180,7 @@
         <v>44</v>
       </c>
       <c r="B86" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C86">
         <f t="shared" si="1"/>
@@ -5240,7 +5228,7 @@
         <v>111</v>
       </c>
       <c r="B87" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C87">
         <f t="shared" si="1"/>
@@ -5288,7 +5276,7 @@
         <v>66</v>
       </c>
       <c r="B88" t="s">
-        <v>231</v>
+        <v>161</v>
       </c>
       <c r="C88">
         <f t="shared" si="1"/>
@@ -5336,7 +5324,7 @@
         <v>139</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C89">
         <f t="shared" si="1"/>
@@ -5384,7 +5372,7 @@
         <v>106</v>
       </c>
       <c r="B90" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C90">
         <f t="shared" si="1"/>
@@ -5432,7 +5420,7 @@
         <v>112</v>
       </c>
       <c r="B91" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C91">
         <f t="shared" si="1"/>

</xml_diff>